<commit_message>
Updated 19th April 2024
</commit_message>
<xml_diff>
--- a/interview/PySpark and SQL.xlsx
+++ b/interview/PySpark and SQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF230EA-1B18-4A60-814A-D3037F45403B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47735E3F-2A75-4CD3-979D-665D3670AE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{9767B20F-FE94-4063-9030-5A036B42D00B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{9767B20F-FE94-4063-9030-5A036B42D00B}"/>
   </bookViews>
   <sheets>
     <sheet name="PySpark" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58171634-9D04-4E2E-B7D4-E27DB372F024}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F92D1B-2915-4F09-93B1-78E57405A681}">
   <dimension ref="C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>